<commit_message>
output excel file is stored here
</commit_message>
<xml_diff>
--- a/outputFiles/Profiles.xlsx
+++ b/outputFiles/Profiles.xlsx
@@ -1,19 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yazee\OneDrive\Documents\Projects and Open Source\chrome-development\linkedin-scraper\outputFiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802C3351-FE85-4FEA-AB45-A6CB449630D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Freelancers" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>linkedin_url</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -50,6 +75,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -374,155 +407,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>name</v>
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
-      <c r="B1" t="str">
-        <v>linkedin_url</v>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
-      <c r="C1" t="str">
-        <v>title</v>
+      <c r="C1" t="s">
+        <v>2</v>
       </c>
-      <c r="D1" t="str">
-        <v>location</v>
+      <c r="D1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Farah Dahabi, LCSW</v>
-      </c>
-      <c r="B2" t="str">
-        <v>https://www.linkedin.com/in/farahbabar/</v>
-      </c>
-      <c r="C2" t="str">
-        <v>Director of Mental Health First Aid UAE (Dual-Licensed in the US &amp; Dubai)</v>
-      </c>
-      <c r="D2" t="str">
-        <v xml:space="preserve">Dubai, United Arab Emirates </v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Frederick J. Bentivegna</v>
-      </c>
-      <c r="B3" t="str">
-        <v>https://www.linkedin.com/in/frederick-j-bentivegna-a74b7726/</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Foremost Pool Scientist of America, Author and Sports Personality</v>
-      </c>
-      <c r="D3" t="str">
-        <v xml:space="preserve">Greater Chicago Area </v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Paul Firth FInstSMM</v>
-      </c>
-      <c r="B4" t="str">
-        <v>https://www.linkedin.com/in/paul-firth-finstsmm-b3578a8/</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Founder &amp; Managing Director - ICAS MENA</v>
-      </c>
-      <c r="D4" t="str">
-        <v xml:space="preserve">United Arab Emirates </v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Federica Polato</v>
-      </c>
-      <c r="B5" t="str">
-        <v>https://www.linkedin.com/in/federica-polato1/</v>
-      </c>
-      <c r="C5" t="str">
-        <v>International Business Consultant</v>
-      </c>
-      <c r="D5" t="str">
-        <v xml:space="preserve">Dubai, United Arab Emirates </v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Renzo Harmse</v>
-      </c>
-      <c r="B6" t="str">
-        <v>https://www.linkedin.com/in/renzo-harmse-894a14bb/</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Jack of all trades, master of Marketing, boss of Business Development, Advertising ninja 😁</v>
-      </c>
-      <c r="D6" t="str">
-        <v xml:space="preserve">Dubai, United Arab Emirates </v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Noel Dias</v>
-      </c>
-      <c r="B7" t="str">
-        <v>https://www.linkedin.com/in/noel-dias-883162160/</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Business Development Executive at HonorFX</v>
-      </c>
-      <c r="D7" t="str">
-        <v xml:space="preserve">United Arab Emirates </v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>SHOAIB AHMED SHARIFF MBA,Cert CII</v>
-      </c>
-      <c r="B8" t="str">
-        <v>https://www.linkedin.com/in/shoaib-ahmed-shariff-mba-cert-cii-72b34817/</v>
-      </c>
-      <c r="C8" t="str">
-        <v>Senior Relationship Manager(Commercial Lines) at Oman Insurance Company</v>
-      </c>
-      <c r="D8" t="str">
-        <v xml:space="preserve">United Arab Emirates </v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>Samy Kw</v>
-      </c>
-      <c r="B9" t="str">
-        <v>https://www.linkedin.com/in/samy-kw-4a7351181/</v>
-      </c>
-      <c r="C9" t="str">
-        <v>Chairman في Biko Digital Marketing</v>
-      </c>
-      <c r="D9" t="str">
-        <v xml:space="preserve">Egypt </v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>sankari Venkateswaran</v>
-      </c>
-      <c r="B10" t="str">
-        <v>https://www.linkedin.com/in/sankari-venkateswaran-0ba329104/</v>
-      </c>
-      <c r="C10" t="str">
-        <v>Business Development Manager at IBM GLOBAL MIDDLE EAST | UAE Company Formation Specialist</v>
-      </c>
-      <c r="D10" t="str">
-        <v xml:space="preserve">Dubai, United Arab Emirates </v>
-      </c>
-    </row>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D10"/>
+    <ignoredError sqref="A1:D1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>